<commit_message>
Añadidos todos los desesperantes intentos fallidos
</commit_message>
<xml_diff>
--- a/Pract2y3/MapasKarnaugh.xlsx
+++ b/Pract2y3/MapasKarnaugh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopez\RepositoriosGithub\EVE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\EVE\Pract2y3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0E5CAA-8DEB-4A4C-BB91-134FB5FD04CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50873966-E888-42AC-BFFA-FFB97A6790BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14430" yWindow="0" windowWidth="14475" windowHeight="15585" xr2:uid="{B734BD75-F41B-4450-B9D1-1F0A51AD3406}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{B734BD75-F41B-4450-B9D1-1F0A51AD3406}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,17 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>D0</t>
   </si>
@@ -90,13 +91,19 @@
   </si>
   <si>
     <t xml:space="preserve">Amarillo bajo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sentido directo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sentido inverso </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1127,16 +1134,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EC99F3-A9F7-4A6A-A723-A526C12991A8}">
-  <dimension ref="B3:W33"/>
+  <dimension ref="B2:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M14" workbookViewId="0">
-      <selection activeCell="W35" sqref="W35"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="3" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:23" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:23">
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" ht="13.9" thickBot="1"/>
+    <row r="4" spans="2:23" ht="30.4" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1192,7 +1207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:23" ht="15.75" thickBot="1">
       <c r="B5" s="4">
         <v>0</v>
       </c>
@@ -1248,7 +1263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23" ht="15.75" thickBot="1">
       <c r="B6" s="7">
         <v>0</v>
       </c>
@@ -1304,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23" ht="15.75" thickBot="1">
       <c r="B7" s="4">
         <v>0</v>
       </c>
@@ -1360,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:23" ht="15.75" thickBot="1">
       <c r="B8" s="7">
         <v>0</v>
       </c>
@@ -1416,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:23" ht="15.75" thickBot="1">
       <c r="B9" s="4">
         <v>1</v>
       </c>
@@ -1472,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:23" ht="15.75" thickBot="1">
       <c r="B10" s="7">
         <v>1</v>
       </c>
@@ -1528,7 +1543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:23" ht="15.75" thickBot="1">
       <c r="B11" s="4">
         <v>1</v>
       </c>
@@ -1584,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:23" ht="15.75" thickBot="1">
       <c r="B12" s="7">
         <v>1</v>
       </c>
@@ -1640,7 +1655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -1660,7 +1675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:23">
       <c r="B33" t="s">
         <v>12</v>
       </c>

</xml_diff>